<commit_message>
successful publishing mazak to umati app
</commit_message>
<xml_diff>
--- a/mtc2umati/mtc2umati/Mapping.xlsx
+++ b/mtc2umati/mtc2umati/Mapping.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalData\arzer\Seafile\Meine Bibliothek\MeineProjekte\umati\connect\mtc2umati\mtc2umati\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalData\arzer\Seafile\Meine Bibliothek\MeineProjekte\umati\net_umaticonnect\mtc2umati\mtc2umati\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1F5A5E-6B03-4CE1-A6B4-3C4CA15CF336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE99F07F-6A89-46D7-96A6-9AB59AC1D709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{C8900138-5871-4382-9539-8E39C53F56A2}"/>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{03908AE4-99AE-4B02-82B0-01AC17757249}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{264555F1-0172-4A46-8607-1BBA516D8533}"/>
+    <workbookView xWindow="-16320" yWindow="-5280" windowWidth="16440" windowHeight="28320" activeTab="1" xr2:uid="{40695492-071F-42C0-91D8-1CF4EDDA561A}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping_DMG" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4620" uniqueCount="709">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4631" uniqueCount="710">
   <si>
     <t>Modelling Rule</t>
   </si>
@@ -3293,13 +3293,16 @@
     <t>RapidOverrideRange</t>
   </si>
   <si>
-    <t>#None</t>
-  </si>
-  <si>
     <t>Program Name</t>
   </si>
   <si>
     <t>Serial Number</t>
+  </si>
+  <si>
+    <t>#N 52.4260022 E 9.6175556</t>
+  </si>
+  <si>
+    <t>#http://mazak.com</t>
   </si>
 </sst>
 </file>
@@ -3943,7 +3946,7 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AE8FAD02-9A69-4F06-801A-E0FFF72BEC0F}" name="Tabelle636" displayName="Tabelle636" ref="A1:L200" totalsRowShown="0">
   <autoFilter ref="A1:L200" xr:uid="{35CFAB4B-0F7E-4FC4-9533-702E35E8C9F1}">
-    <filterColumn colId="11">
+    <filterColumn colId="7">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
@@ -4372,8 +4375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86714E06-43CE-41D1-B0FA-37CA50D75756}">
   <dimension ref="A1:N150"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="C70" workbookViewId="0">
+      <selection activeCell="D94" sqref="D94"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -4730,6 +4733,15 @@
       <c r="F14" s="8" t="s">
         <v>22</v>
       </c>
+      <c r="G14" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>708</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="K14" s="13"/>
       <c r="M14" s="15"/>
       <c r="N14" s="15"/>
@@ -7906,12 +7918,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84283000-7D10-4DA9-8365-BFFC6E636655}">
   <dimension ref="A1:L200"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView topLeftCell="C133" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H186" sqref="H186"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="C106" workbookViewId="1">
-      <selection activeCell="G131" sqref="G131"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9065,10 +9075,16 @@
       <c r="F38" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
+      <c r="G38" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H38" s="18" t="s">
+        <v>708</v>
+      </c>
       <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
+      <c r="J38" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
     </row>
@@ -9272,7 +9288,7 @@
         <v>22</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H45" s="8" t="s">
         <v>678</v>
@@ -12228,10 +12244,13 @@
         <v>22</v>
       </c>
       <c r="G172" s="8" t="s">
-        <v>707</v>
-      </c>
-      <c r="H172" s="8" t="s">
-        <v>679</v>
+        <v>706</v>
+      </c>
+      <c r="H172" s="9" t="s">
+        <v>473</v>
+      </c>
+      <c r="I172" s="8" t="s">
+        <v>571</v>
       </c>
       <c r="J172" s="8" t="s">
         <v>21</v>
@@ -12432,6 +12451,9 @@
       <c r="H180" s="9" t="s">
         <v>483</v>
       </c>
+      <c r="J180" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="K180" s="8" t="s">
         <v>484</v>
       </c>
@@ -12509,9 +12531,6 @@
       </c>
       <c r="G183" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="H183" s="8" t="s">
-        <v>706</v>
       </c>
       <c r="J183" s="8" t="s">
         <v>21</v>
@@ -12917,8 +12936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA108938-A41A-4607-947C-EAC9A8B9EE57}">
   <dimension ref="A1:L200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D173" sqref="D173"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -12978,7 +12997,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>92</v>
       </c>
@@ -13008,7 +13027,7 @@
       </c>
       <c r="L2" s="32"/>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>92</v>
       </c>
@@ -13038,7 +13057,7 @@
       </c>
       <c r="L3" s="32"/>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>311</v>
       </c>
@@ -13068,7 +13087,7 @@
       </c>
       <c r="L4" s="32"/>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>92</v>
       </c>
@@ -13098,7 +13117,7 @@
       </c>
       <c r="L5" s="32"/>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>311</v>
       </c>
@@ -13128,7 +13147,7 @@
       </c>
       <c r="L6" s="32"/>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>92</v>
       </c>
@@ -13158,7 +13177,7 @@
       </c>
       <c r="L7" s="32"/>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>92</v>
       </c>
@@ -13188,7 +13207,7 @@
       </c>
       <c r="L8" s="32"/>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>311</v>
       </c>
@@ -13218,7 +13237,7 @@
       </c>
       <c r="L9" s="32"/>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>92</v>
       </c>
@@ -13248,7 +13267,7 @@
       </c>
       <c r="L10" s="32"/>
     </row>
-    <row r="11" spans="1:12" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>311</v>
       </c>
@@ -13278,7 +13297,7 @@
       </c>
       <c r="L11" s="33"/>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>311</v>
       </c>
@@ -13308,7 +13327,7 @@
       </c>
       <c r="L12" s="32"/>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>311</v>
       </c>
@@ -13338,7 +13357,7 @@
       </c>
       <c r="L13" s="32"/>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>92</v>
       </c>
@@ -13368,7 +13387,7 @@
       </c>
       <c r="L14" s="32"/>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>92</v>
       </c>
@@ -13398,7 +13417,7 @@
       </c>
       <c r="L15" s="32"/>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>311</v>
       </c>
@@ -13428,7 +13447,7 @@
       </c>
       <c r="L16" s="32"/>
     </row>
-    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>92</v>
       </c>
@@ -13458,7 +13477,7 @@
       </c>
       <c r="L17" s="32"/>
     </row>
-    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>311</v>
       </c>
@@ -13488,7 +13507,7 @@
       </c>
       <c r="L18" s="32"/>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>92</v>
       </c>
@@ -13518,7 +13537,7 @@
       </c>
       <c r="L19" s="32"/>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>92</v>
       </c>
@@ -13548,7 +13567,7 @@
       </c>
       <c r="L20" s="32"/>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>311</v>
       </c>
@@ -13578,7 +13597,7 @@
       </c>
       <c r="L21" s="32"/>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>92</v>
       </c>
@@ -13608,7 +13627,7 @@
       </c>
       <c r="L22" s="32"/>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>311</v>
       </c>
@@ -13638,7 +13657,7 @@
       </c>
       <c r="L23" s="32"/>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>92</v>
       </c>
@@ -13668,7 +13687,7 @@
       </c>
       <c r="L24" s="32"/>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>311</v>
       </c>
@@ -13698,7 +13717,7 @@
       </c>
       <c r="L25" s="32"/>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>311</v>
       </c>
@@ -13728,7 +13747,7 @@
       </c>
       <c r="L26" s="32"/>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>92</v>
       </c>
@@ -13758,7 +13777,7 @@
       </c>
       <c r="L27" s="32"/>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>311</v>
       </c>
@@ -13863,7 +13882,7 @@
       </c>
       <c r="L32" s="32"/>
     </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>14</v>
       </c>
@@ -13980,26 +13999,35 @@
       </c>
       <c r="L37" s="32"/>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" s="8" t="s">
+    <row r="38" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="E38" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L38" s="32"/>
+      <c r="E38" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G38" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="H38" s="18" t="s">
+        <v>708</v>
+      </c>
+      <c r="J38" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L38" s="34"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
@@ -14054,7 +14082,7 @@
       </c>
       <c r="L40" s="32"/>
     </row>
-    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>14</v>
       </c>
@@ -14152,7 +14180,7 @@
         <v>32</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>677</v>
+        <v>709</v>
       </c>
       <c r="J44" s="8" t="s">
         <v>21</v>
@@ -14211,7 +14239,7 @@
       </c>
       <c r="L46" s="32"/>
     </row>
-    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>92</v>
       </c>
@@ -14244,7 +14272,7 @@
       </c>
       <c r="L47" s="32"/>
     </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>311</v>
       </c>
@@ -14280,7 +14308,7 @@
       </c>
       <c r="L48" s="32"/>
     </row>
-    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>92</v>
       </c>
@@ -14334,7 +14362,7 @@
       </c>
       <c r="L50" s="32"/>
     </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>92</v>
       </c>
@@ -14367,7 +14395,7 @@
       </c>
       <c r="L51" s="32"/>
     </row>
-    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>311</v>
       </c>
@@ -14403,7 +14431,7 @@
       </c>
       <c r="L52" s="32"/>
     </row>
-    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>92</v>
       </c>
@@ -14579,7 +14607,7 @@
       </c>
       <c r="L60" s="32"/>
     </row>
-    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>179</v>
       </c>
@@ -14609,7 +14637,7 @@
       </c>
       <c r="L61" s="32"/>
     </row>
-    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
         <v>179</v>
       </c>
@@ -14643,7 +14671,7 @@
       </c>
       <c r="L62" s="32"/>
     </row>
-    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>179</v>
       </c>
@@ -14744,7 +14772,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
         <v>179</v>
       </c>
@@ -16133,7 +16161,7 @@
       </c>
       <c r="L129" s="32"/>
     </row>
-    <row r="130" spans="1:12" ht="43.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="8" t="s">
         <v>10</v>
       </c>
@@ -16187,7 +16215,7 @@
       </c>
       <c r="L131" s="32"/>
     </row>
-    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="8" t="s">
         <v>311</v>
       </c>
@@ -16217,7 +16245,7 @@
       </c>
       <c r="L132" s="32"/>
     </row>
-    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="8" t="s">
         <v>311</v>
       </c>
@@ -16251,7 +16279,7 @@
       <c r="K133" s="9"/>
       <c r="L133" s="32"/>
     </row>
-    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" s="8" t="s">
         <v>311</v>
       </c>
@@ -16285,7 +16313,7 @@
       <c r="K134" s="9"/>
       <c r="L134" s="32"/>
     </row>
-    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="8" t="s">
         <v>311</v>
       </c>
@@ -16318,7 +16346,7 @@
       </c>
       <c r="L135" s="32"/>
     </row>
-    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="8" t="s">
         <v>311</v>
       </c>
@@ -16351,7 +16379,7 @@
       </c>
       <c r="L136" s="32"/>
     </row>
-    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="8" t="s">
         <v>311</v>
       </c>
@@ -16727,7 +16755,7 @@
       </c>
       <c r="L154" s="32"/>
     </row>
-    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" s="8" t="s">
         <v>311</v>
       </c>
@@ -16760,7 +16788,7 @@
       </c>
       <c r="L155" s="32"/>
     </row>
-    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" s="8" t="s">
         <v>311</v>
       </c>
@@ -16790,7 +16818,7 @@
       </c>
       <c r="L156" s="32"/>
     </row>
-    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" s="8" t="s">
         <v>311</v>
       </c>
@@ -16821,7 +16849,7 @@
       <c r="K157" s="9"/>
       <c r="L157" s="32"/>
     </row>
-    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" s="8" t="s">
         <v>311</v>
       </c>
@@ -16854,7 +16882,7 @@
       </c>
       <c r="L158" s="32"/>
     </row>
-    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" s="8" t="s">
         <v>311</v>
       </c>
@@ -16902,7 +16930,7 @@
       </c>
       <c r="L160" s="32"/>
     </row>
-    <row r="161" spans="1:12" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="15" t="s">
         <v>179</v>
       </c>
@@ -17049,7 +17077,7 @@
       </c>
       <c r="L167" s="32"/>
     </row>
-    <row r="168" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A168" s="8" t="s">
         <v>179</v>
       </c>
@@ -17082,7 +17110,7 @@
       </c>
       <c r="L168" s="32"/>
     </row>
-    <row r="169" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A169" s="8" t="s">
         <v>14</v>
       </c>
@@ -17136,7 +17164,7 @@
       </c>
       <c r="L170" s="32"/>
     </row>
-    <row r="171" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A171" s="8" t="s">
         <v>311</v>
       </c>
@@ -17166,7 +17194,7 @@
       </c>
       <c r="L171" s="32"/>
     </row>
-    <row r="172" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A172" s="8" t="s">
         <v>10</v>
       </c>
@@ -17228,7 +17256,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A174" s="8" t="s">
         <v>179</v>
       </c>
@@ -17261,7 +17289,7 @@
       </c>
       <c r="L174" s="32"/>
     </row>
-    <row r="175" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A175" s="8" t="s">
         <v>311</v>
       </c>
@@ -17369,7 +17397,7 @@
       </c>
       <c r="L179" s="32"/>
     </row>
-    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A180" s="8" t="s">
         <v>10</v>
       </c>
@@ -17393,6 +17421,9 @@
       </c>
       <c r="H180" s="9" t="s">
         <v>483</v>
+      </c>
+      <c r="J180" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="K180" s="8" t="s">
         <v>484</v>
@@ -17634,7 +17665,7 @@
       </c>
       <c r="L190" s="32"/>
     </row>
-    <row r="191" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A191" s="8" t="s">
         <v>311</v>
       </c>
@@ -17668,7 +17699,7 @@
       </c>
       <c r="L191" s="32"/>
     </row>
-    <row r="192" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A192" s="8" t="s">
         <v>311</v>
       </c>
@@ -17702,7 +17733,7 @@
       </c>
       <c r="L192" s="32"/>
     </row>
-    <row r="193" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A193" s="8" t="s">
         <v>311</v>
       </c>
@@ -17735,7 +17766,7 @@
       </c>
       <c r="L193" s="32"/>
     </row>
-    <row r="194" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A194" s="8" t="s">
         <v>311</v>
       </c>
@@ -17840,7 +17871,7 @@
       </c>
       <c r="L198" s="32"/>
     </row>
-    <row r="199" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A199" s="8" t="s">
         <v>311</v>
       </c>
@@ -17889,9 +17920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAAAFC79-5577-476B-B1CC-67E10685991A}">
   <dimension ref="B2:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17955,9 +17984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A74275F-88CC-4439-9C7E-3B35A97F1CB9}">
   <dimension ref="A1:D123"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19692,9 +19719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F71650-1B07-47D5-BD9D-8CEDD8564375}">
   <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20739,9 +20764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{916638A0-997A-4DC7-9F1B-B62E0940B85E}">
   <dimension ref="B3:AD54"/>
   <sheetViews>
-    <sheetView topLeftCell="N24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AJ43" sqref="AJ43"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
working publishing to umati app
</commit_message>
<xml_diff>
--- a/mtc2umati/mtc2umati/Mapping.xlsx
+++ b/mtc2umati/mtc2umati/Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalData\arzer\Seafile\Meine Bibliothek\MeineProjekte\umati\connect\mtc2umati\mtc2umati\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D202F1-BE4E-4236-AF26-A48FDBD26C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95FF7256-1463-49A0-B7FF-648D691AB020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{40695492-071F-42C0-91D8-1CF4EDDA561A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{40695492-071F-42C0-91D8-1CF4EDDA561A}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping_DMG" sheetId="9" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4657" uniqueCount="712">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4667" uniqueCount="712">
   <si>
     <t>Modelling Rule</t>
   </si>
@@ -3504,7 +3504,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3579,6 +3579,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -8017,8 +8018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84283000-7D10-4DA9-8365-BFFC6E636655}">
   <dimension ref="A1:L200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B88" workbookViewId="0">
-      <selection activeCell="H111" sqref="H111"/>
+    <sheetView topLeftCell="B88" workbookViewId="0">
+      <selection activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13026,8 +13027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA108938-A41A-4607-947C-EAC9A8B9EE57}">
   <dimension ref="A1:L200"/>
   <sheetViews>
-    <sheetView topLeftCell="C160" workbookViewId="0">
-      <selection activeCell="F188" sqref="F188"/>
+    <sheetView tabSelected="1" topLeftCell="B61" workbookViewId="0">
+      <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15067,70 +15068,98 @@
       <c r="G72" s="15"/>
       <c r="L72" s="32"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A73" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B73" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C73" s="8" t="s">
+    <row r="73" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B73" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C73" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="D73" s="8" t="s">
+      <c r="D73" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="E73" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F73" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L73" s="32"/>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A74" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B74" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C74" s="8" t="s">
+      <c r="E73" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="F73" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G73" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="H73" s="41" t="s">
+        <v>426</v>
+      </c>
+      <c r="I73" s="37" t="s">
+        <v>427</v>
+      </c>
+      <c r="J73" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="L73" s="40"/>
+    </row>
+    <row r="74" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B74" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C74" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="D74" s="8" t="s">
+      <c r="D74" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="E74" s="8" t="s">
+      <c r="E74" s="37" t="s">
         <v>697</v>
       </c>
-      <c r="F74" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G74" s="7"/>
-      <c r="L74" s="32"/>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A75" s="8" t="s">
+      <c r="F74" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G74" s="42" t="s">
+        <v>702</v>
+      </c>
+      <c r="H74" s="37" t="s">
+        <v>698</v>
+      </c>
+      <c r="J74" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="L74" s="40"/>
+    </row>
+    <row r="75" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="B75" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C75" s="8" t="s">
+      <c r="B75" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C75" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="D75" s="8" t="s">
+      <c r="D75" s="37" t="s">
         <v>696</v>
       </c>
-      <c r="E75" s="8" t="s">
+      <c r="E75" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="F75" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G75" s="7"/>
-      <c r="L75" s="32"/>
+      <c r="F75" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G75" s="42" t="s">
+        <v>703</v>
+      </c>
+      <c r="H75" s="37" t="s">
+        <v>699</v>
+      </c>
+      <c r="J75" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="L75" s="40"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
@@ -20863,13 +20892,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="45" t="s">
         <v>640</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
       <c r="G3" s="10" t="s">
         <v>641</v>
       </c>
@@ -20902,13 +20931,13 @@
       <c r="AD3" s="5"/>
     </row>
     <row r="4" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="46" t="s">
         <v>644</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
       <c r="G4" s="11" t="s">
         <v>645</v>
       </c>
@@ -20941,34 +20970,34 @@
       <c r="AD4" s="11"/>
     </row>
     <row r="6" spans="2:30" s="2" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="44" t="s">
         <v>648</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="M6" s="43" t="s">
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="M6" s="44" t="s">
         <v>649</v>
       </c>
-      <c r="N6" s="43"/>
-      <c r="O6" s="43"/>
-      <c r="P6" s="43"/>
-      <c r="Q6" s="43"/>
-      <c r="R6" s="43"/>
-      <c r="S6" s="43"/>
-      <c r="T6" s="43"/>
-      <c r="W6" s="43" t="s">
+      <c r="N6" s="44"/>
+      <c r="O6" s="44"/>
+      <c r="P6" s="44"/>
+      <c r="Q6" s="44"/>
+      <c r="R6" s="44"/>
+      <c r="S6" s="44"/>
+      <c r="T6" s="44"/>
+      <c r="W6" s="44" t="s">
         <v>650</v>
       </c>
-      <c r="X6" s="43"/>
-      <c r="Y6" s="43"/>
-      <c r="Z6" s="43"/>
-      <c r="AA6" s="43"/>
-      <c r="AB6" s="43"/>
-      <c r="AC6" s="43"/>
+      <c r="X6" s="44"/>
+      <c r="Y6" s="44"/>
+      <c r="Z6" s="44"/>
+      <c r="AA6" s="44"/>
+      <c r="AB6" s="44"/>
+      <c r="AC6" s="44"/>
     </row>
     <row r="7" spans="2:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
@@ -21002,260 +21031,260 @@
       <c r="AD7" s="5"/>
     </row>
     <row r="24" spans="13:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M24" s="42" t="s">
+      <c r="M24" s="43" t="s">
         <v>651</v>
       </c>
-      <c r="N24" s="42"/>
-      <c r="O24" s="42"/>
-      <c r="P24" s="42"/>
-      <c r="Q24" s="42"/>
-      <c r="R24" s="42"/>
-      <c r="S24" s="42"/>
-      <c r="T24" s="42"/>
+      <c r="N24" s="43"/>
+      <c r="O24" s="43"/>
+      <c r="P24" s="43"/>
+      <c r="Q24" s="43"/>
+      <c r="R24" s="43"/>
+      <c r="S24" s="43"/>
+      <c r="T24" s="43"/>
     </row>
     <row r="25" spans="13:20" x14ac:dyDescent="0.25">
-      <c r="M25" s="42"/>
-      <c r="N25" s="42"/>
-      <c r="O25" s="42"/>
-      <c r="P25" s="42"/>
-      <c r="Q25" s="42"/>
-      <c r="R25" s="42"/>
-      <c r="S25" s="42"/>
-      <c r="T25" s="42"/>
+      <c r="M25" s="43"/>
+      <c r="N25" s="43"/>
+      <c r="O25" s="43"/>
+      <c r="P25" s="43"/>
+      <c r="Q25" s="43"/>
+      <c r="R25" s="43"/>
+      <c r="S25" s="43"/>
+      <c r="T25" s="43"/>
     </row>
     <row r="26" spans="13:20" x14ac:dyDescent="0.25">
-      <c r="M26" s="42"/>
-      <c r="N26" s="42"/>
-      <c r="O26" s="42"/>
-      <c r="P26" s="42"/>
-      <c r="Q26" s="42"/>
-      <c r="R26" s="42"/>
-      <c r="S26" s="42"/>
-      <c r="T26" s="42"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="43"/>
+      <c r="P26" s="43"/>
+      <c r="Q26" s="43"/>
+      <c r="R26" s="43"/>
+      <c r="S26" s="43"/>
+      <c r="T26" s="43"/>
     </row>
     <row r="27" spans="13:20" x14ac:dyDescent="0.25">
-      <c r="M27" s="42"/>
-      <c r="N27" s="42"/>
-      <c r="O27" s="42"/>
-      <c r="P27" s="42"/>
-      <c r="Q27" s="42"/>
-      <c r="R27" s="42"/>
-      <c r="S27" s="42"/>
-      <c r="T27" s="42"/>
+      <c r="M27" s="43"/>
+      <c r="N27" s="43"/>
+      <c r="O27" s="43"/>
+      <c r="P27" s="43"/>
+      <c r="Q27" s="43"/>
+      <c r="R27" s="43"/>
+      <c r="S27" s="43"/>
+      <c r="T27" s="43"/>
     </row>
     <row r="28" spans="13:20" x14ac:dyDescent="0.25">
-      <c r="M28" s="42"/>
-      <c r="N28" s="42"/>
-      <c r="O28" s="42"/>
-      <c r="P28" s="42"/>
-      <c r="Q28" s="42"/>
-      <c r="R28" s="42"/>
-      <c r="S28" s="42"/>
-      <c r="T28" s="42"/>
+      <c r="M28" s="43"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="43"/>
+      <c r="P28" s="43"/>
+      <c r="Q28" s="43"/>
+      <c r="R28" s="43"/>
+      <c r="S28" s="43"/>
+      <c r="T28" s="43"/>
     </row>
     <row r="29" spans="13:20" x14ac:dyDescent="0.25">
-      <c r="M29" s="42"/>
-      <c r="N29" s="42"/>
-      <c r="O29" s="42"/>
-      <c r="P29" s="42"/>
-      <c r="Q29" s="42"/>
-      <c r="R29" s="42"/>
-      <c r="S29" s="42"/>
-      <c r="T29" s="42"/>
+      <c r="M29" s="43"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="43"/>
+      <c r="P29" s="43"/>
+      <c r="Q29" s="43"/>
+      <c r="R29" s="43"/>
+      <c r="S29" s="43"/>
+      <c r="T29" s="43"/>
     </row>
     <row r="30" spans="13:20" x14ac:dyDescent="0.25">
-      <c r="M30" s="42"/>
-      <c r="N30" s="42"/>
-      <c r="O30" s="42"/>
-      <c r="P30" s="42"/>
-      <c r="Q30" s="42"/>
-      <c r="R30" s="42"/>
-      <c r="S30" s="42"/>
-      <c r="T30" s="42"/>
+      <c r="M30" s="43"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="43"/>
+      <c r="P30" s="43"/>
+      <c r="Q30" s="43"/>
+      <c r="R30" s="43"/>
+      <c r="S30" s="43"/>
+      <c r="T30" s="43"/>
     </row>
     <row r="31" spans="13:20" x14ac:dyDescent="0.25">
-      <c r="M31" s="42"/>
-      <c r="N31" s="42"/>
-      <c r="O31" s="42"/>
-      <c r="P31" s="42"/>
-      <c r="Q31" s="42"/>
-      <c r="R31" s="42"/>
-      <c r="S31" s="42"/>
-      <c r="T31" s="42"/>
+      <c r="M31" s="43"/>
+      <c r="N31" s="43"/>
+      <c r="O31" s="43"/>
+      <c r="P31" s="43"/>
+      <c r="Q31" s="43"/>
+      <c r="R31" s="43"/>
+      <c r="S31" s="43"/>
+      <c r="T31" s="43"/>
     </row>
     <row r="32" spans="13:20" ht="134.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M32" s="42"/>
-      <c r="N32" s="42"/>
-      <c r="O32" s="42"/>
-      <c r="P32" s="42"/>
-      <c r="Q32" s="42"/>
-      <c r="R32" s="42"/>
-      <c r="S32" s="42"/>
-      <c r="T32" s="42"/>
+      <c r="M32" s="43"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="43"/>
+      <c r="P32" s="43"/>
+      <c r="Q32" s="43"/>
+      <c r="R32" s="43"/>
+      <c r="S32" s="43"/>
+      <c r="T32" s="43"/>
     </row>
     <row r="37" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="42" t="s">
+      <c r="B37" s="43" t="s">
         <v>652</v>
       </c>
-      <c r="C37" s="42"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="42"/>
-      <c r="G37" s="42"/>
-      <c r="H37" s="42"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="43"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="43"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="42"/>
-      <c r="C38" s="42"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="42"/>
-      <c r="F38" s="42"/>
-      <c r="G38" s="42"/>
-      <c r="H38" s="42"/>
+      <c r="B38" s="43"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="43"/>
+      <c r="E38" s="43"/>
+      <c r="F38" s="43"/>
+      <c r="G38" s="43"/>
+      <c r="H38" s="43"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="42"/>
-      <c r="C39" s="42"/>
-      <c r="D39" s="42"/>
-      <c r="E39" s="42"/>
-      <c r="F39" s="42"/>
-      <c r="G39" s="42"/>
-      <c r="H39" s="42"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="43"/>
+      <c r="D39" s="43"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="43"/>
+      <c r="H39" s="43"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="42"/>
-      <c r="C40" s="42"/>
-      <c r="D40" s="42"/>
-      <c r="E40" s="42"/>
-      <c r="F40" s="42"/>
-      <c r="G40" s="42"/>
-      <c r="H40" s="42"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="43"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="42"/>
-      <c r="C41" s="42"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="42"/>
-      <c r="F41" s="42"/>
-      <c r="G41" s="42"/>
-      <c r="H41" s="42"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="43"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="43"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="43"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="42"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="42"/>
-      <c r="F42" s="42"/>
-      <c r="G42" s="42"/>
-      <c r="H42" s="42"/>
+      <c r="B42" s="43"/>
+      <c r="C42" s="43"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="43"/>
+      <c r="F42" s="43"/>
+      <c r="G42" s="43"/>
+      <c r="H42" s="43"/>
     </row>
     <row r="43" spans="2:8" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="42"/>
-      <c r="C43" s="42"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="42"/>
-      <c r="F43" s="42"/>
-      <c r="G43" s="42"/>
-      <c r="H43" s="42"/>
+      <c r="B43" s="43"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="43"/>
+      <c r="G43" s="43"/>
+      <c r="H43" s="43"/>
     </row>
     <row r="44" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="42"/>
-      <c r="C44" s="42"/>
-      <c r="D44" s="42"/>
-      <c r="E44" s="42"/>
-      <c r="F44" s="42"/>
-      <c r="G44" s="42"/>
-      <c r="H44" s="42"/>
+      <c r="B44" s="43"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="43"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="43"/>
+      <c r="G44" s="43"/>
+      <c r="H44" s="43"/>
     </row>
     <row r="45" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="42"/>
-      <c r="C45" s="42"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="42"/>
-      <c r="F45" s="42"/>
-      <c r="G45" s="42"/>
-      <c r="H45" s="42"/>
+      <c r="B45" s="43"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="43"/>
+      <c r="E45" s="43"/>
+      <c r="F45" s="43"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="43"/>
     </row>
     <row r="46" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="42"/>
-      <c r="C46" s="42"/>
-      <c r="D46" s="42"/>
-      <c r="E46" s="42"/>
-      <c r="F46" s="42"/>
-      <c r="G46" s="42"/>
-      <c r="H46" s="42"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="43"/>
+      <c r="E46" s="43"/>
+      <c r="F46" s="43"/>
+      <c r="G46" s="43"/>
+      <c r="H46" s="43"/>
     </row>
     <row r="47" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="42"/>
-      <c r="C47" s="42"/>
-      <c r="D47" s="42"/>
-      <c r="E47" s="42"/>
-      <c r="F47" s="42"/>
-      <c r="G47" s="42"/>
-      <c r="H47" s="42"/>
+      <c r="B47" s="43"/>
+      <c r="C47" s="43"/>
+      <c r="D47" s="43"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="43"/>
+      <c r="G47" s="43"/>
+      <c r="H47" s="43"/>
     </row>
     <row r="48" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="42"/>
-      <c r="C48" s="42"/>
-      <c r="D48" s="42"/>
-      <c r="E48" s="42"/>
-      <c r="F48" s="42"/>
-      <c r="G48" s="42"/>
-      <c r="H48" s="42"/>
+      <c r="B48" s="43"/>
+      <c r="C48" s="43"/>
+      <c r="D48" s="43"/>
+      <c r="E48" s="43"/>
+      <c r="F48" s="43"/>
+      <c r="G48" s="43"/>
+      <c r="H48" s="43"/>
     </row>
     <row r="49" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="42"/>
-      <c r="C49" s="42"/>
-      <c r="D49" s="42"/>
-      <c r="E49" s="42"/>
-      <c r="F49" s="42"/>
-      <c r="G49" s="42"/>
-      <c r="H49" s="42"/>
+      <c r="B49" s="43"/>
+      <c r="C49" s="43"/>
+      <c r="D49" s="43"/>
+      <c r="E49" s="43"/>
+      <c r="F49" s="43"/>
+      <c r="G49" s="43"/>
+      <c r="H49" s="43"/>
     </row>
     <row r="50" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="42"/>
-      <c r="C50" s="42"/>
-      <c r="D50" s="42"/>
-      <c r="E50" s="42"/>
-      <c r="F50" s="42"/>
-      <c r="G50" s="42"/>
-      <c r="H50" s="42"/>
+      <c r="B50" s="43"/>
+      <c r="C50" s="43"/>
+      <c r="D50" s="43"/>
+      <c r="E50" s="43"/>
+      <c r="F50" s="43"/>
+      <c r="G50" s="43"/>
+      <c r="H50" s="43"/>
     </row>
     <row r="51" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="42"/>
-      <c r="C51" s="42"/>
-      <c r="D51" s="42"/>
-      <c r="E51" s="42"/>
-      <c r="F51" s="42"/>
-      <c r="G51" s="42"/>
-      <c r="H51" s="42"/>
+      <c r="B51" s="43"/>
+      <c r="C51" s="43"/>
+      <c r="D51" s="43"/>
+      <c r="E51" s="43"/>
+      <c r="F51" s="43"/>
+      <c r="G51" s="43"/>
+      <c r="H51" s="43"/>
     </row>
     <row r="52" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="42"/>
-      <c r="C52" s="42"/>
-      <c r="D52" s="42"/>
-      <c r="E52" s="42"/>
-      <c r="F52" s="42"/>
-      <c r="G52" s="42"/>
-      <c r="H52" s="42"/>
+      <c r="B52" s="43"/>
+      <c r="C52" s="43"/>
+      <c r="D52" s="43"/>
+      <c r="E52" s="43"/>
+      <c r="F52" s="43"/>
+      <c r="G52" s="43"/>
+      <c r="H52" s="43"/>
     </row>
     <row r="53" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="42"/>
-      <c r="C53" s="42"/>
-      <c r="D53" s="42"/>
-      <c r="E53" s="42"/>
-      <c r="F53" s="42"/>
-      <c r="G53" s="42"/>
-      <c r="H53" s="42"/>
+      <c r="B53" s="43"/>
+      <c r="C53" s="43"/>
+      <c r="D53" s="43"/>
+      <c r="E53" s="43"/>
+      <c r="F53" s="43"/>
+      <c r="G53" s="43"/>
+      <c r="H53" s="43"/>
     </row>
     <row r="54" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="42"/>
-      <c r="C54" s="42"/>
-      <c r="D54" s="42"/>
-      <c r="E54" s="42"/>
-      <c r="F54" s="42"/>
-      <c r="G54" s="42"/>
-      <c r="H54" s="42"/>
+      <c r="B54" s="43"/>
+      <c r="C54" s="43"/>
+      <c r="D54" s="43"/>
+      <c r="E54" s="43"/>
+      <c r="F54" s="43"/>
+      <c r="G54" s="43"/>
+      <c r="H54" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
mazak umati app fully featured
</commit_message>
<xml_diff>
--- a/mtc2umati/mtc2umati/Mapping.xlsx
+++ b/mtc2umati/mtc2umati/Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalData\arzer\Seafile\Meine Bibliothek\MeineProjekte\umati\connect\mtc2umati\mtc2umati\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95FF7256-1463-49A0-B7FF-648D691AB020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76146CC-99F4-49BB-8784-A2D4E031F82E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{40695492-071F-42C0-91D8-1CF4EDDA561A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4667" uniqueCount="712">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4683" uniqueCount="723">
   <si>
     <t>Modelling Rule</t>
   </si>
@@ -3309,6 +3309,39 @@
   <si>
     <t>EURange</t>
   </si>
+  <si>
+    <t>#Showroom Machine</t>
+  </si>
+  <si>
+    <t>#HB07HA0012E</t>
+  </si>
+  <si>
+    <t>#1.3.0.17</t>
+  </si>
+  <si>
+    <t>#2018</t>
+  </si>
+  <si>
+    <t>#Showcase_MPF</t>
+  </si>
+  <si>
+    <t>#Axis Mill</t>
+  </si>
+  <si>
+    <t>e.g. "AUTOMATIC", "MANUAL_DATA_INPUT"</t>
+  </si>
+  <si>
+    <t>Monitoring/MachineTool/OperationDuration</t>
+  </si>
+  <si>
+    <t>Controller/controller/AccumulatedTime</t>
+  </si>
+  <si>
+    <t>In seconds, but total time</t>
+  </si>
+  <si>
+    <t>x:TOTAL</t>
+  </si>
 </sst>
 </file>
 
@@ -3930,10 +3963,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{09AB0687-0850-4689-9112-8648F9A75ED2}" name="Tabelle635" displayName="Tabelle635" ref="A1:K150" totalsRowShown="0">
-  <autoFilter ref="A1:K150" xr:uid="{35CFAB4B-0F7E-4FC4-9533-702E35E8C9F1}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K150">
-    <sortCondition ref="D1:D150"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{09AB0687-0850-4689-9112-8648F9A75ED2}" name="Tabelle635" displayName="Tabelle635" ref="A1:K149" totalsRowShown="0">
+  <autoFilter ref="A1:K149" xr:uid="{35CFAB4B-0F7E-4FC4-9533-702E35E8C9F1}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K149">
+    <sortCondition ref="D1:D149"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{D697A07D-8E3E-4E31-BAF7-7B83F7F8171B}" name="Modelling Rule"/>
@@ -4400,10 +4433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86714E06-43CE-41D1-B0FA-37CA50D75756}">
-  <dimension ref="A1:N150"/>
+  <dimension ref="A1:N149"/>
   <sheetViews>
-    <sheetView topLeftCell="E22" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40:D52"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6506,7 +6539,7 @@
         <v>259</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>260</v>
+        <v>719</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>188</v>
@@ -6556,14 +6589,14 @@
       <c r="A89" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B89" s="8" t="s">
+      <c r="B89" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C89" s="8" t="s">
         <v>186</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>187</v>
+        <v>429</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>188</v>
@@ -6571,120 +6604,128 @@
       <c r="F89" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K89" s="13"/>
+      <c r="G89" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="H89" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="J89" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="K89" s="13" t="s">
+        <v>263</v>
+      </c>
       <c r="M89" s="15"/>
       <c r="N89" s="15"/>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B90" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B90" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>186</v>
+        <v>71</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>188</v>
+        <v>73</v>
       </c>
       <c r="F90" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G90" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="H90" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="J90" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="K90" s="13" t="s">
-        <v>263</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="K90" s="13"/>
       <c r="M90" s="15"/>
       <c r="N90" s="15"/>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B91" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B91" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>71</v>
+        <v>190</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>73</v>
+        <v>192</v>
       </c>
       <c r="F91" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="K91" s="13"/>
+        <v>103</v>
+      </c>
+      <c r="G91" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="H91" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="J91" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K91" s="14" t="s">
+        <v>661</v>
+      </c>
       <c r="M91" s="15"/>
       <c r="N91" s="15"/>
     </row>
-    <row r="92" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B92" s="12" t="s">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="E92" s="8" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="F92" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="G92" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="H92" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="J92" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K92" s="14" t="s">
-        <v>661</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="K92" s="13"/>
       <c r="M92" s="15"/>
       <c r="N92" s="15"/>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>11</v>
+        <v>92</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>198</v>
+        <v>289</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>199</v>
+        <v>290</v>
+      </c>
+      <c r="E93" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="F93" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="K93" s="13"/>
-      <c r="M93" s="15"/>
-      <c r="N93" s="15"/>
+        <v>103</v>
+      </c>
+      <c r="G93" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="H93" s="8" t="s">
+        <v>673</v>
+      </c>
+      <c r="I93" s="8"/>
+      <c r="J93" s="8"/>
+      <c r="K93" s="8" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="94" spans="1:14" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
@@ -6694,30 +6735,32 @@
         <v>18</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>21</v>
+        <v>102</v>
       </c>
       <c r="F94" s="8" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="G94" s="8" t="s">
         <v>291</v>
       </c>
       <c r="H94" s="8" t="s">
-        <v>673</v>
+        <v>292</v>
       </c>
       <c r="I94" s="8"/>
-      <c r="J94" s="8"/>
+      <c r="J94" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="K94" s="8" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="95" spans="1:14" s="15" customFormat="1" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
         <v>92</v>
       </c>
@@ -6725,29 +6768,25 @@
         <v>18</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="F95" s="8" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="G95" s="8" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="H95" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="I95" s="8"/>
-      <c r="J95" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K95" s="8" t="s">
-        <v>298</v>
+        <v>674</v>
+      </c>
+      <c r="K95" s="13" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
@@ -6758,25 +6797,28 @@
         <v>18</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>21</v>
+        <v>102</v>
       </c>
       <c r="F96" s="8" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="G96" s="8" t="s">
         <v>300</v>
       </c>
       <c r="H96" s="8" t="s">
-        <v>674</v>
+        <v>301</v>
+      </c>
+      <c r="J96" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="K96" s="13" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
@@ -6787,28 +6829,25 @@
         <v>18</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="F97" s="8" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="G97" s="8" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="H97" s="8" t="s">
-        <v>301</v>
-      </c>
-      <c r="J97" s="8" t="s">
-        <v>21</v>
+        <v>675</v>
       </c>
       <c r="K97" s="13" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
@@ -6819,25 +6858,28 @@
         <v>18</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>21</v>
+        <v>102</v>
       </c>
       <c r="F98" s="8" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="G98" s="8" t="s">
         <v>304</v>
       </c>
       <c r="H98" s="8" t="s">
-        <v>675</v>
+        <v>305</v>
+      </c>
+      <c r="J98" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="K98" s="13" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
@@ -6848,28 +6890,25 @@
         <v>18</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="F99" s="8" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="G99" s="8" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="H99" s="8" t="s">
-        <v>305</v>
-      </c>
-      <c r="J99" s="8" t="s">
-        <v>21</v>
+        <v>676</v>
       </c>
       <c r="K99" s="13" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
@@ -6880,92 +6919,84 @@
         <v>18</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>21</v>
+        <v>102</v>
       </c>
       <c r="F100" s="8" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="G100" s="8" t="s">
         <v>308</v>
       </c>
       <c r="H100" s="8" t="s">
-        <v>676</v>
+        <v>309</v>
+      </c>
+      <c r="J100" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="K100" s="13" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B101" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B101" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>296</v>
+        <v>19</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>310</v>
+        <v>201</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="F101" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G101" s="8" t="s">
-        <v>308</v>
-      </c>
-      <c r="H101" s="8" t="s">
-        <v>309</v>
-      </c>
-      <c r="J101" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K101" s="13" t="s">
-        <v>298</v>
-      </c>
+      <c r="K101" s="13"/>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B102" s="4" t="s">
-        <v>18</v>
+        <v>202</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>19</v>
+        <v>203</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="E102" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F102" s="8" t="s">
-        <v>22</v>
+        <v>204</v>
       </c>
       <c r="K102" s="13"/>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
-        <v>202</v>
+        <v>92</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>204</v>
+        <v>206</v>
+      </c>
+      <c r="E103" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="F103" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="K103" s="13"/>
     </row>
@@ -6977,55 +7008,55 @@
         <v>18</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="E104" s="8" t="s">
-        <v>178</v>
+        <v>214</v>
       </c>
       <c r="F104" s="8" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="K104" s="13"/>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="E105" s="8" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="F105" s="8" t="s">
-        <v>103</v>
+        <v>224</v>
       </c>
       <c r="K105" s="13"/>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="8" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>223</v>
+        <v>226</v>
+      </c>
+      <c r="E106" s="8" t="s">
+        <v>227</v>
       </c>
       <c r="F106" s="8" t="s">
-        <v>224</v>
+        <v>103</v>
       </c>
       <c r="K106" s="13"/>
     </row>
@@ -7037,37 +7068,37 @@
         <v>18</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="E107" s="8" t="s">
-        <v>227</v>
+        <v>197</v>
       </c>
       <c r="F107" s="8" t="s">
-        <v>103</v>
+        <v>230</v>
       </c>
       <c r="K107" s="13"/>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="B108" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>228</v>
+        <v>87</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="E108" s="8" t="s">
-        <v>197</v>
+        <v>21</v>
       </c>
       <c r="F108" s="8" t="s">
-        <v>230</v>
+        <v>22</v>
       </c>
       <c r="K108" s="13"/>
     </row>
@@ -7079,13 +7110,13 @@
         <v>18</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E109" s="8" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="F109" s="8" t="s">
         <v>22</v>
@@ -7094,19 +7125,19 @@
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="8" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="B110" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E110" s="8" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="F110" s="8" t="s">
         <v>22</v>
@@ -7115,16 +7146,16 @@
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="8" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="B111" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E111" s="8" t="s">
         <v>95</v>
@@ -7142,13 +7173,13 @@
         <v>18</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E112" s="8" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F112" s="8" t="s">
         <v>22</v>
@@ -7157,193 +7188,190 @@
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="8" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="B113" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>98</v>
+        <v>236</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="E113" s="8" t="s">
-        <v>85</v>
+        <v>238</v>
       </c>
       <c r="F113" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K113" s="13"/>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="8" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="E114" s="8" t="s">
-        <v>238</v>
+        <v>102</v>
       </c>
       <c r="F114" s="8" t="s">
-        <v>22</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="K114" s="13"/>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="8" t="s">
-        <v>14</v>
+        <v>311</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>239</v>
+        <v>312</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>240</v>
+        <v>313</v>
       </c>
       <c r="E115" s="8" t="s">
-        <v>102</v>
+        <v>31</v>
       </c>
       <c r="F115" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="K115" s="13"/>
+        <v>103</v>
+      </c>
+      <c r="G115" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="H115" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="J115" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K115" s="13" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="8" t="s">
-        <v>311</v>
+        <v>179</v>
       </c>
       <c r="B116" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>313</v>
+        <v>654</v>
       </c>
       <c r="E116" s="8" t="s">
-        <v>31</v>
+        <v>102</v>
       </c>
       <c r="F116" s="8" t="s">
         <v>103</v>
       </c>
       <c r="G116" s="8" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="H116" s="8" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="J116" s="8" t="s">
         <v>21</v>
       </c>
       <c r="K116" s="13" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="8" t="s">
-        <v>179</v>
+        <v>10</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>316</v>
+        <v>242</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>654</v>
-      </c>
-      <c r="E117" s="8" t="s">
-        <v>102</v>
+        <v>242</v>
       </c>
       <c r="F117" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="G117" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="H117" s="8" t="s">
-        <v>318</v>
-      </c>
-      <c r="J117" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K117" s="13" t="s">
-        <v>319</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="K117" s="13"/>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B118" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C118" s="8" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="F118" s="8" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="K118" s="13"/>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="8" t="s">
-        <v>14</v>
+        <v>311</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C119" s="8" t="s">
-        <v>244</v>
+        <v>332</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>245</v>
+        <v>653</v>
+      </c>
+      <c r="E119" s="8" t="s">
+        <v>197</v>
       </c>
       <c r="F119" s="8" t="s">
-        <v>246</v>
+        <v>103</v>
+      </c>
+      <c r="G119" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="H119" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="J119" s="8" t="s">
+        <v>197</v>
       </c>
       <c r="K119" s="13"/>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="8" t="s">
-        <v>311</v>
+        <v>14</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C120" s="8" t="s">
-        <v>332</v>
+        <v>247</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>653</v>
-      </c>
-      <c r="E120" s="8" t="s">
-        <v>197</v>
+        <v>248</v>
       </c>
       <c r="F120" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="G120" s="8" t="s">
-        <v>332</v>
-      </c>
-      <c r="H120" s="9" t="s">
-        <v>333</v>
-      </c>
-      <c r="J120" s="8" t="s">
-        <v>197</v>
+        <v>249</v>
       </c>
       <c r="K120" s="13"/>
     </row>
@@ -7351,38 +7379,38 @@
       <c r="A121" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B121" s="8" t="s">
-        <v>11</v>
+      <c r="B121" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>247</v>
+        <v>19</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>248</v>
+        <v>250</v>
+      </c>
+      <c r="E121" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="F121" s="8" t="s">
-        <v>249</v>
+        <v>22</v>
       </c>
       <c r="K121" s="13"/>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B122" s="12" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="C122" s="8" t="s">
-        <v>19</v>
+        <v>251</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="E122" s="8" t="s">
-        <v>21</v>
+        <v>251</v>
       </c>
       <c r="F122" s="8" t="s">
-        <v>22</v>
+        <v>252</v>
       </c>
       <c r="K122" s="13"/>
     </row>
@@ -7394,31 +7422,40 @@
         <v>11</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="F123" s="8" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="K123" s="13"/>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="8" t="s">
-        <v>10</v>
+        <v>179</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>253</v>
+        <v>320</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>254</v>
+        <v>321</v>
+      </c>
+      <c r="E124" s="8" t="s">
+        <v>123</v>
       </c>
       <c r="F124" s="8" t="s">
-        <v>255</v>
+        <v>103</v>
+      </c>
+      <c r="G124" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="H124" s="9" t="s">
+        <v>322</v>
       </c>
       <c r="K124" s="13"/>
     </row>
@@ -7430,10 +7467,10 @@
         <v>18</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="E125" s="8" t="s">
         <v>123</v>
@@ -7442,40 +7479,43 @@
         <v>103</v>
       </c>
       <c r="G125" s="8" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="H125" s="9" t="s">
-        <v>322</v>
+        <v>326</v>
+      </c>
+      <c r="I125" s="9" t="s">
+        <v>327</v>
       </c>
       <c r="K125" s="13"/>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="B126" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B126" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="E126" s="8" t="s">
-        <v>123</v>
+        <v>21</v>
       </c>
       <c r="F126" s="8" t="s">
         <v>103</v>
       </c>
       <c r="G126" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="H126" s="9" t="s">
-        <v>326</v>
-      </c>
-      <c r="I126" s="9" t="s">
-        <v>327</v>
+        <v>330</v>
+      </c>
+      <c r="H126" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="J126" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="K126" s="13"/>
     </row>
@@ -7487,46 +7527,46 @@
         <v>18</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>328</v>
+        <v>264</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>329</v>
+        <v>265</v>
       </c>
       <c r="E127" s="8" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="F127" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="G127" s="8" t="s">
-        <v>330</v>
-      </c>
-      <c r="H127" s="8" t="s">
-        <v>331</v>
-      </c>
-      <c r="J127" s="8" t="s">
-        <v>21</v>
-      </c>
       <c r="K127" s="13"/>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B128" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>264</v>
+        <v>36</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="E128" s="8" t="s">
-        <v>109</v>
+        <v>21</v>
       </c>
       <c r="F128" s="8" t="s">
-        <v>103</v>
+        <v>22</v>
+      </c>
+      <c r="G128" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="H128" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="J128" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="K128" s="13"/>
     </row>
@@ -7538,117 +7578,107 @@
         <v>18</v>
       </c>
       <c r="C129" s="8" t="s">
-        <v>36</v>
+        <v>257</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="E129" s="8" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="F129" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="G129" s="8" t="s">
-        <v>330</v>
-      </c>
-      <c r="H129" s="8" t="s">
-        <v>331</v>
-      </c>
-      <c r="J129" s="8" t="s">
-        <v>21</v>
       </c>
       <c r="K129" s="13"/>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B130" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="B130" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>257</v>
+        <v>334</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>258</v>
+        <v>335</v>
       </c>
       <c r="E130" s="8" t="s">
-        <v>77</v>
+        <v>123</v>
       </c>
       <c r="F130" s="8" t="s">
-        <v>22</v>
+        <v>103</v>
+      </c>
+      <c r="G130" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="H130" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="I130" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="J130" s="8" t="s">
+        <v>197</v>
       </c>
       <c r="K130" s="13"/>
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="8" t="s">
-        <v>311</v>
+        <v>179</v>
       </c>
       <c r="B131" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C131" s="8" t="s">
-        <v>334</v>
+        <v>294</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>335</v>
+        <v>295</v>
       </c>
       <c r="E131" s="8" t="s">
-        <v>123</v>
+        <v>21</v>
       </c>
       <c r="F131" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="G131" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="H131" s="9" t="s">
-        <v>326</v>
-      </c>
-      <c r="I131" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="J131" s="8" t="s">
-        <v>197</v>
-      </c>
       <c r="K131" s="13"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A132" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="B132" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C132" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="D132" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="E132" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F132" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="K132" s="13"/>
+    <row r="132" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B132" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C132" s="37" t="s">
+        <v>266</v>
+      </c>
+      <c r="D132" s="37" t="s">
+        <v>267</v>
+      </c>
+      <c r="K132" s="38"/>
     </row>
     <row r="133" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="B133" s="37" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="B133" s="39" t="s">
+        <v>18</v>
       </c>
       <c r="C133" s="37" t="s">
-        <v>266</v>
+        <v>107</v>
       </c>
       <c r="D133" s="37" t="s">
-        <v>267</v>
-      </c>
-      <c r="K133" s="38"/>
+        <v>268</v>
+      </c>
+      <c r="E133" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="F133" s="37" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="134" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="37" t="s">
@@ -7658,10 +7688,10 @@
         <v>18</v>
       </c>
       <c r="C134" s="37" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D134" s="37" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E134" s="37" t="s">
         <v>109</v>
@@ -7672,120 +7702,120 @@
     </row>
     <row r="135" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="37" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B135" s="39" t="s">
         <v>18</v>
       </c>
       <c r="C135" s="37" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D135" s="37" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E135" s="37" t="s">
-        <v>109</v>
+        <v>31</v>
       </c>
       <c r="F135" s="37" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="136" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="B136" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="C136" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="D136" s="37" t="s">
-        <v>270</v>
-      </c>
-      <c r="E136" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="G135" s="37" t="s">
+        <v>482</v>
+      </c>
+      <c r="H135" s="41" t="s">
+        <v>633</v>
+      </c>
+      <c r="J135" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="K135" s="37" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A136" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B136" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C136" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D136" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="E136" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F136" s="37" t="s">
-        <v>114</v>
-      </c>
-      <c r="G136" s="37" t="s">
-        <v>482</v>
-      </c>
-      <c r="H136" s="41" t="s">
-        <v>633</v>
-      </c>
-      <c r="J136" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="K136" s="37" t="s">
-        <v>484</v>
+      <c r="F136" s="8" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B137" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C137" s="8" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E137" s="8" t="s">
-        <v>31</v>
+        <v>109</v>
       </c>
       <c r="F137" s="8" t="s">
         <v>22</v>
+      </c>
+      <c r="G137" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H137" s="8" t="s">
+        <v>679</v>
+      </c>
+      <c r="J137" s="9" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B138" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C138" s="8" t="s">
-        <v>117</v>
+        <v>36</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="E138" s="8" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="F138" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="G138" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="H138" s="8" t="s">
-        <v>679</v>
-      </c>
-      <c r="J138" s="9" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B139" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C139" s="8" t="s">
-        <v>36</v>
+        <v>121</v>
       </c>
       <c r="D139" s="8" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E139" s="8" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="F139" s="8" t="s">
         <v>22</v>
@@ -7793,22 +7823,22 @@
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B140" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C140" s="8" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D140" s="8" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="E140" s="8" t="s">
-        <v>123</v>
+        <v>31</v>
       </c>
       <c r="F140" s="8" t="s">
-        <v>22</v>
+        <v>126</v>
       </c>
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.25">
@@ -7819,16 +7849,16 @@
         <v>18</v>
       </c>
       <c r="C141" s="8" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E141" s="8" t="s">
-        <v>31</v>
+        <v>129</v>
       </c>
       <c r="F141" s="8" t="s">
-        <v>126</v>
+        <v>22</v>
       </c>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.25">
@@ -7839,13 +7869,13 @@
         <v>18</v>
       </c>
       <c r="C142" s="8" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E142" s="8" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="F142" s="8" t="s">
         <v>22</v>
@@ -7859,13 +7889,13 @@
         <v>18</v>
       </c>
       <c r="C143" s="8" t="s">
-        <v>117</v>
+        <v>36</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E143" s="8" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="F143" s="8" t="s">
         <v>22</v>
@@ -7879,13 +7909,13 @@
         <v>18</v>
       </c>
       <c r="C144" s="8" t="s">
-        <v>36</v>
+        <v>121</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E144" s="8" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="F144" s="8" t="s">
         <v>22</v>
@@ -7899,13 +7929,13 @@
         <v>18</v>
       </c>
       <c r="C145" s="8" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E145" s="8" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="F145" s="8" t="s">
         <v>22</v>
@@ -7919,16 +7949,16 @@
         <v>18</v>
       </c>
       <c r="C146" s="8" t="s">
-        <v>133</v>
+        <v>183</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="E146" s="8" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F146" s="8" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
@@ -7936,19 +7966,16 @@
         <v>14</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C147" s="8" t="s">
-        <v>183</v>
+        <v>281</v>
       </c>
       <c r="D147" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="E147" s="8" t="s">
-        <v>123</v>
+        <v>282</v>
       </c>
       <c r="F147" s="8" t="s">
-        <v>103</v>
+        <v>283</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
@@ -7956,16 +7983,19 @@
         <v>14</v>
       </c>
       <c r="B148" s="8" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C148" s="8" t="s">
-        <v>281</v>
+        <v>19</v>
       </c>
       <c r="D148" s="8" t="s">
         <v>282</v>
       </c>
+      <c r="E148" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="F148" s="8" t="s">
-        <v>283</v>
+        <v>22</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
@@ -7973,32 +8003,12 @@
         <v>14</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C149" s="8" t="s">
-        <v>19</v>
+        <v>284</v>
       </c>
       <c r="D149" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="E149" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F149" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A150" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B150" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C150" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="D150" s="8" t="s">
         <v>285</v>
       </c>
     </row>
@@ -13027,8 +13037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA108938-A41A-4607-947C-EAC9A8B9EE57}">
   <dimension ref="A1:L200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B61" workbookViewId="0">
-      <selection activeCell="E79" sqref="E79"/>
+    <sheetView tabSelected="1" topLeftCell="E115" workbookViewId="0">
+      <selection activeCell="I137" sqref="I137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14045,7 +14055,18 @@
       <c r="F35" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="L35" s="32"/>
+      <c r="G35" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>717</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L35" s="32" t="s">
+        <v>688</v>
+      </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
@@ -14117,7 +14138,9 @@
       <c r="J38" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="L38" s="34"/>
+      <c r="L38" s="34" t="s">
+        <v>688</v>
+      </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
@@ -14245,7 +14268,18 @@
       <c r="F43" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="L43" s="32"/>
+      <c r="G43" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>712</v>
+      </c>
+      <c r="J43" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L43" s="32" t="s">
+        <v>688</v>
+      </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
@@ -14302,7 +14336,7 @@
         <v>51</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>678</v>
+        <v>713</v>
       </c>
       <c r="J45" s="8" t="s">
         <v>21</v>
@@ -14635,7 +14669,18 @@
       <c r="F57" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="L57" s="32"/>
+      <c r="G57" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H57" s="8" t="s">
+        <v>714</v>
+      </c>
+      <c r="J57" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L57" s="32" t="s">
+        <v>688</v>
+      </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
@@ -14677,7 +14722,18 @@
       <c r="F59" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="L59" s="32"/>
+      <c r="G59" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H59" s="8" t="s">
+        <v>715</v>
+      </c>
+      <c r="J59" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L59" s="32" t="s">
+        <v>688</v>
+      </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
@@ -14757,7 +14813,7 @@
         <v>21</v>
       </c>
       <c r="K62" s="8" t="s">
-        <v>425</v>
+        <v>718</v>
       </c>
       <c r="L62" s="32"/>
     </row>
@@ -16332,6 +16388,21 @@
       <c r="F131" s="8" t="s">
         <v>103</v>
       </c>
+      <c r="G131" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="H131" s="8" t="s">
+        <v>720</v>
+      </c>
+      <c r="I131" s="8" t="s">
+        <v>722</v>
+      </c>
+      <c r="J131" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K131" s="8" t="s">
+        <v>721</v>
+      </c>
       <c r="L131" s="32"/>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.25">
@@ -17339,7 +17410,7 @@
         <v>682</v>
       </c>
       <c r="H172" s="8" t="s">
-        <v>679</v>
+        <v>716</v>
       </c>
       <c r="J172" s="8" t="s">
         <v>21</v>

</xml_diff>